<commit_message>
1)objectRepoCreated 2)Writing Data into excel file class created
</commit_message>
<xml_diff>
--- a/advanced_selenium_a30/src/test/resources/ExcelFile.xlsx
+++ b/advanced_selenium_a30/src/test/resources/ExcelFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\eclipse-workspace\TestNG Workspace\advanced_selenium_a30\src\test\resources\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>TC_ID</t>
   </si>
@@ -62,12 +62,19 @@
   </si>
   <si>
     <t>qsp_01</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,12 +429,12 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
     </row>
@@ -446,33 +453,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="20.88671875"/>
+    <col min="3" max="3" customWidth="true" width="22.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>